<commit_message>
Fixed when zero remain was counted as changed
Fixed error in output if there were no changed days
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!_DEVELOPMENT\GitHub\WorkTimeCalculator-ExcelAddIn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C81A46F-AFE8-4BDB-9097-BEABDFEE9385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBF1766-7C71-458F-88BA-2B1E0CE0C29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D308C395-0972-4EC3-A0B6-CFFD6257D50A}"/>
   </bookViews>
@@ -56,21 +56,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>1,0=145,12</t>
-  </si>
-  <si>
-    <t>1x5</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Врачи</t>
   </si>
   <si>
-    <t>2*5</t>
+    <t>1,0=72,36</t>
   </si>
   <si>
-    <t>3х5</t>
+    <t>5x5</t>
   </si>
 </sst>
 </file>
@@ -423,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB444B9-E656-4202-9E0C-E04F784DDC39}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,49 +430,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="str" cm="1">
-        <f t="array" ref="A4:A5">_xll.WorkTime($B1,A3,$C1,$A1)</f>
-        <v>21x6.22</v>
-      </c>
-      <c r="B4" t="str" cm="1">
-        <f t="array" ref="B4:B5">_xll.WorkTime($B1,B3,$C1,$A1)</f>
-        <v>21x6.8</v>
-      </c>
-      <c r="C4" t="str" cm="1">
-        <f t="array" ref="C4:C5">_xll.WorkTime($B1,C3,$C1,$A1)</f>
-        <v>21x5.55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="str">
-        <v>1x6.30</v>
-      </c>
-      <c r="B5" t="str">
-        <v>1x6.24</v>
-      </c>
-      <c r="C5" t="str">
-        <v>1x5.57</v>
+        <f t="array" ref="A4">_xll.WorkTime($B1,A3,$C1,$A1)</f>
+        <v>8x5.57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Check max time for employee
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!_DEVELOPMENT\GitHub\WorkTimeCalculator-ExcelAddIn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBF1766-7C71-458F-88BA-2B1E0CE0C29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F419014A-7873-4A20-A597-CE98AC1B751A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D308C395-0972-4EC3-A0B6-CFFD6257D50A}"/>
   </bookViews>
@@ -56,15 +56,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Врачи</t>
-  </si>
-  <si>
-    <t>1,0=72,36</t>
-  </si>
-  <si>
-    <t>5x5</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>0x0</t>
+  </si>
+  <si>
+    <t>3x8</t>
+  </si>
+  <si>
+    <t>5x8</t>
+  </si>
+  <si>
+    <t>4x5</t>
+  </si>
+  <si>
+    <t>Средний медперсонал</t>
+  </si>
+  <si>
+    <t>1x9</t>
+  </si>
+  <si>
+    <t>1,0=148,12</t>
+  </si>
+  <si>
+    <t>2x9</t>
   </si>
 </sst>
 </file>
@@ -417,41 +432,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB444B9-E656-4202-9E0C-E04F784DDC39}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str" cm="1">
         <f t="array" ref="A4">_xll.WorkTime($B1,A3,$C1,$A1)</f>
-        <v>8x5.57</v>
+        <v>19x7,48</v>
+      </c>
+      <c r="B4" t="str" cm="1">
+        <f t="array" ref="B4:B5">_xll.WorkTime($B1,B3,$C1,$A1)</f>
+        <v>18x7,19</v>
+      </c>
+      <c r="C4" t="str" cm="1">
+        <f t="array" ref="C4:C5">_xll.WorkTime($B1,C3,$C1,$A1)</f>
+        <v>18x6,51</v>
+      </c>
+      <c r="D4" t="str" cm="1">
+        <f t="array" ref="D4:D5">_xll.WorkTime($B1,D3,$C1,$A1)</f>
+        <v>18x6,32</v>
+      </c>
+      <c r="E4" t="str" cm="1">
+        <f t="array" ref="E4:E5">_xll.WorkTime($B1,E3,$C1,$A1)</f>
+        <v>18x6,44</v>
+      </c>
+      <c r="F4" t="str" cm="1">
+        <f t="array" ref="F4:F5">_xll.WorkTime($B1,F3,$C1,$A1)</f>
+        <v>18x5,41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
+        <v>1x7,30</v>
+      </c>
+      <c r="C5" t="str">
+        <v>1x6,54</v>
+      </c>
+      <c r="D5" t="str">
+        <v>1x6,36</v>
+      </c>
+      <c r="E5" t="str">
+        <v>1x7,0</v>
+      </c>
+      <c r="F5" t="str">
+        <v>1x5,54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A4" evalError="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
QoL Middle Employee Input String
</commit_message>
<xml_diff>
--- a/Example.xlsx
+++ b/Example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!_DEVELOPMENT\GitHub\WorkTimeCalculator-ExcelAddIn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\!_DEVELOPMENT\!_GITHUB\WorkTimeCalculator-ExcelAddIn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F419014A-7873-4A20-A597-CE98AC1B751A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E482E132-378A-4F2E-894A-7F7A24450B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D308C395-0972-4EC3-A0B6-CFFD6257D50A}"/>
   </bookViews>
@@ -56,30 +56,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>0x0</t>
   </si>
   <si>
-    <t>3x8</t>
+    <t>1,0=156,0</t>
   </si>
   <si>
-    <t>5x8</t>
-  </si>
-  <si>
-    <t>4x5</t>
-  </si>
-  <si>
-    <t>Средний медперсонал</t>
-  </si>
-  <si>
-    <t>1x9</t>
-  </si>
-  <si>
-    <t>1,0=148,12</t>
-  </si>
-  <si>
-    <t>2x9</t>
+    <t>Средний</t>
   </si>
 </sst>
 </file>
@@ -432,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB444B9-E656-4202-9E0C-E04F784DDC39}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,76 +431,69 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2</v>
+      <c r="B3" t="str">
+        <f>_xlfn.CONCAT("1х",A7)</f>
+        <v>1х5</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xlfn.CONCAT("2х",A7)</f>
+        <v>2х5</v>
+      </c>
+      <c r="D3" t="str">
+        <f>_xlfn.CONCAT("3х",A7)</f>
+        <v>3х5</v>
+      </c>
+      <c r="E3" t="str">
+        <f>_xlfn.CONCAT("4х",A7)</f>
+        <v>4х5</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xlfn.CONCAT("5х",A7)</f>
+        <v>5х5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str" cm="1">
         <f t="array" ref="A4">_xll.WorkTime($B1,A3,$C1,$A1)</f>
-        <v>19x7,48</v>
+        <v>20x7,48</v>
       </c>
       <c r="B4" t="str" cm="1">
-        <f t="array" ref="B4:B5">_xll.WorkTime($B1,B3,$C1,$A1)</f>
-        <v>18x7,19</v>
+        <f t="array" ref="B4">_xll.WorkTime($B1,B3,$C1,$A1)</f>
+        <v>20x7,33</v>
       </c>
       <c r="C4" t="str" cm="1">
-        <f t="array" ref="C4:C5">_xll.WorkTime($B1,C3,$C1,$A1)</f>
-        <v>18x6,51</v>
+        <f t="array" ref="C4">_xll.WorkTime($B1,C3,$C1,$A1)</f>
+        <v>20x7,18</v>
       </c>
       <c r="D4" t="str" cm="1">
-        <f t="array" ref="D4:D5">_xll.WorkTime($B1,D3,$C1,$A1)</f>
-        <v>18x6,32</v>
+        <f t="array" ref="D4">_xll.WorkTime($B1,D3,$C1,$A1)</f>
+        <v>20x7,3</v>
       </c>
       <c r="E4" t="str" cm="1">
-        <f t="array" ref="E4:E5">_xll.WorkTime($B1,E3,$C1,$A1)</f>
-        <v>18x6,44</v>
+        <f t="array" ref="E4">_xll.WorkTime($B1,E3,$C1,$A1)</f>
+        <v>20x6,48</v>
       </c>
       <c r="F4" t="str" cm="1">
-        <f t="array" ref="F4:F5">_xll.WorkTime($B1,F3,$C1,$A1)</f>
-        <v>18x5,41</v>
+        <f t="array" ref="F4">_xll.WorkTime($B1,F3,$C1,$A1)</f>
+        <v>20x6,33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="str">
-        <v>1x7,30</v>
-      </c>
-      <c r="C5" t="str">
-        <v>1x6,54</v>
-      </c>
-      <c r="D5" t="str">
-        <v>1x6,36</v>
-      </c>
-      <c r="E5" t="str">
-        <v>1x7,0</v>
-      </c>
-      <c r="F5" t="str">
-        <v>1x5,54</v>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>